<commit_message>
Add GitHub Personal Access Token asset to config files
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71439B22-4E38-4C8D-955B-38292DF03730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>GitCredentials</t>
+  </si>
+  <si>
+    <t>Git Credentials</t>
+  </si>
+  <si>
+    <t>P3 Automation</t>
+  </si>
+  <si>
+    <t>QC GitHub Personal Access Token</t>
   </si>
 </sst>
 </file>
@@ -2683,7 +2695,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2730,7 +2742,20 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add queue name and path for input data workbook to config
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71439B22-4E38-4C8D-955B-38292DF03730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986FC932-D1E9-467A-966D-E08CADD72198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -134,6 +130,18 @@
   </si>
   <si>
     <t>QC GitHub Personal Access Token</t>
+  </si>
+  <si>
+    <t>InputDataPath</t>
+  </si>
+  <si>
+    <t>UserGithub</t>
+  </si>
+  <si>
+    <t>D:\Revature\Revature-Capstone-1362\Mock Data.xlsx</t>
+  </si>
+  <si>
+    <t>Path to file with input data.</t>
   </si>
 </sst>
 </file>
@@ -511,14 +519,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -559,16 +567,26 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
@@ -577,7 +595,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1636,7 +1654,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1660,7 +1678,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1682,7 +1700,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1693,7 +1711,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1704,7 +1722,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2694,7 +2712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -2714,7 +2732,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2744,16 +2762,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Setting up Initialization state
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://revaturetech-my.sharepoint.com/personal/frankline295_revature_net/Documents/Revature/frankhume/track-commit-history/CommitTrackerDispatcher/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDFFC6EF-197E-47AE-9F10-CAFE16FD4B71}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1350" yWindow="2850" windowWidth="15510" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -90,10 +90,6 @@
     <t>Framework</t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -123,12 +119,27 @@
   <si>
     <t>OrchestratorAssetFolder</t>
   </si>
+  <si>
+    <t>Git Credentials</t>
+  </si>
+  <si>
+    <t>UserGithub</t>
+  </si>
+  <si>
+    <t>C:\Users\hello2\OneDrive - Revature LLC\Revature\frankhume\track-commit-history\CommitTrackerDispatcher\Mock_Data.xlsx</t>
+  </si>
+  <si>
+    <t>Workbook Name. The path of the workbook name must match with the workbook path in the UiPath studio property.</t>
+  </si>
+  <si>
+    <t>InputDataPath</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +163,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF464E55"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -173,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,6 +200,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -547,13 +565,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -565,10 +583,20 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1624,7 +1652,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1648,7 +1676,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1670,7 +1698,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1681,7 +1709,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1692,7 +1720,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2682,8 +2710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2702,7 +2730,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2730,7 +2758,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3732,5 +3767,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove credential asset from config
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986FC932-D1E9-467A-966D-E08CADD72198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE48C58B-EC91-46CA-8C90-8BA7E8CD72B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="2085" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -118,18 +118,6 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>GitCredentials</t>
-  </si>
-  <si>
-    <t>Git Credentials</t>
-  </si>
-  <si>
-    <t>P3 Automation</t>
-  </si>
-  <si>
-    <t>QC GitHub Personal Access Token</t>
   </si>
   <si>
     <t>InputDataPath</t>
@@ -519,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -570,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -578,13 +566,13 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">
@@ -2712,8 +2700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2760,20 +2748,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add items to queue
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project 3\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE48C58B-EC91-46CA-8C90-8BA7E8CD72B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA453A-B910-4D9F-A483-6EF55F1188F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="2085" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1598" yWindow="1605" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -126,10 +126,10 @@
     <t>UserGithub</t>
   </si>
   <si>
-    <t>D:\Revature\Revature-Capstone-1362\Mock Data.xlsx</t>
+    <t>Path to file with input data.</t>
   </si>
   <si>
-    <t>Path to file with input data.</t>
+    <t>C:\Users\Diaha\Downloads\Mock_Data.xlsx</t>
   </si>
 </sst>
 </file>
@@ -507,16 +507,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.59765625" customWidth="1"/>
+    <col min="2" max="2" width="49.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.3984375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -569,13 +569,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.5">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1592,12 +1592,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.3984375" customWidth="1"/>
+    <col min="4" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1634,7 +1634,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2700,16 +2700,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" customWidth="1"/>
+    <col min="3" max="3" width="60.265625" customWidth="1"/>
+    <col min="4" max="26" width="65.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Clean up activities and use directory path to allow for multiple input files
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project 3\track-commit-history\CommitTrackerDispatcher\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAA453A-B910-4D9F-A483-6EF55F1188F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4083399-AEF2-4C36-A5CF-C4E373BC6C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1598" yWindow="1605" windowWidth="16875" windowHeight="10523" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23355" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Path to file with input data.</t>
-  </si>
-  <si>
-    <t>C:\Users\Diaha\Downloads\Mock_Data.xlsx</t>
   </si>
 </sst>
 </file>
@@ -508,15 +505,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.59765625" customWidth="1"/>
-    <col min="2" max="2" width="49.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -568,14 +565,11 @@
       <c r="A3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="28.5">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1592,12 +1586,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.3984375" customWidth="1"/>
-    <col min="4" max="26" width="8.73046875" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1634,7 +1628,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.5">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2704,12 +2698,12 @@
       <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" customWidth="1"/>
-    <col min="3" max="3" width="60.265625" customWidth="1"/>
-    <col min="4" max="26" width="65.3984375" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Use orchestrator queue name in config
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4083399-AEF2-4C36-A5CF-C4E373BC6C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EAD99A-9F5F-451F-B0ED-095913C5E0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23355" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26955" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -123,10 +123,10 @@
     <t>InputDataPath</t>
   </si>
   <si>
-    <t>UserGithub</t>
+    <t>Path to file with input data.</t>
   </si>
   <si>
-    <t>Path to file with input data.</t>
+    <t>CommitHistoryQueue</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -566,7 +566,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">

</xml_diff>

<commit_message>
Allow custom output path to be set for generated reports
</commit_message>
<xml_diff>
--- a/CommitTrackerDispatcher/Data/Config.xlsx
+++ b/CommitTrackerDispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Revature\Revature-Capstone-1362\track-commit-history\CommitTrackerDispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EAD99A-9F5F-451F-B0ED-095913C5E0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1ED527-DB0F-495D-8FB0-8B9A77A575DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26955" yWindow="3735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23715" yWindow="2205" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -123,10 +123,10 @@
     <t>InputDataPath</t>
   </si>
   <si>
-    <t>Path to file with input data.</t>
+    <t>CommitHistoryQueue</t>
   </si>
   <si>
-    <t>CommitHistoryQueue</t>
+    <t>Path to directory with input files.</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -555,7 +555,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -566,7 +566,7 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="30">

</xml_diff>